<commit_message>
add WELCOME key for MIQ /2
</commit_message>
<xml_diff>
--- a/data_raw/ids_listening_tests.xlsx
+++ b/data_raw/ids_listening_tests.xlsx
@@ -1268,10 +1268,10 @@
     <t xml:space="preserve">AMIQ_0001_I_0032_1</t>
   </si>
   <si>
-    <t xml:space="preserve">Willkommen beim visuellen Puzzletest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Welcome to the Visual Puzzles Test</t>
+    <t xml:space="preserve">Willkommen beim visuellen Puzzletest!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Welcome to the Visual Puzzles Test!</t>
   </si>
   <si>
     <t xml:space="preserve">AMPT_0001_I_0001_1</t>
@@ -7438,8 +7438,8 @@
   </sheetPr>
   <dimension ref="A1:E1032"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C35" activeCellId="0" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.86328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>